<commit_message>
fix var and add template for dhcpscopes
</commit_message>
<xml_diff>
--- a/Powershell/Document_Templates/dhcpreservations.xlsx
+++ b/Powershell/Document_Templates/dhcpreservations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bryank12gaus-my.sharepoint.com/personal/cvincent_bryan_k12_ga_us/Documents/Documents/GitHub/Book-of-Spells/Powershell/Document_Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D67ACA-DCF9-4530-AEF4-95A4EF3FE38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{85D67ACA-DCF9-4530-AEF4-95A4EF3FE38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CB98F3C-428C-4903-A4E5-3EF6E398B174}"/>
   <bookViews>
-    <workbookView xWindow="5565" yWindow="2970" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,25 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>bcboe-fs2</t>
-  </si>
-  <si>
-    <t>10.6.36.0</t>
-  </si>
-  <si>
-    <t>10.6.36.10</t>
-  </si>
-  <si>
-    <t>sip-t54w</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>805e0c78bf38</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>DHCPServer</t>
   </si>
@@ -51,16 +33,19 @@
     <t>ScopeID</t>
   </si>
   <si>
-    <t>IPAddress</t>
-  </si>
-  <si>
-    <t>Hostname</t>
-  </si>
-  <si>
-    <t>ClientID</t>
-  </si>
-  <si>
-    <t>Description</t>
+    <t>StartRange</t>
+  </si>
+  <si>
+    <t>EndRange</t>
+  </si>
+  <si>
+    <t>Router</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>SubnetMask</t>
   </si>
 </sst>
 </file>
@@ -378,60 +363,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>